<commit_message>
(#91) solved multi-operation under one op name problem; generate structured json files for ImageJ library
</commit_message>
<xml_diff>
--- a/mapping_common_input_java_types_full.xlsx
+++ b/mapping_common_input_java_types_full.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\59803\Auto_generation_pipeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EBD9E2E-ECCB-4826-ACD4-7EBFC6DFCFA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DD732D-D111-4EF6-8A49-F7849EF2E151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,12 +16,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="62">
   <si>
     <t>datatype</t>
   </si>
@@ -192,6 +191,21 @@
   </si>
   <si>
     <t>FinalDimensions(x, y)</t>
+  </si>
+  <si>
+    <t>bool_para</t>
+  </si>
+  <si>
+    <t>float_para</t>
+  </si>
+  <si>
+    <t>str_para</t>
+  </si>
+  <si>
+    <t>int_para</t>
+  </si>
+  <si>
+    <t>list_para</t>
   </si>
 </sst>
 </file>
@@ -307,7 +321,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -319,13 +333,13 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -635,7 +649,7 @@
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -682,7 +696,7 @@
         <v>36</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>40</v>
@@ -702,7 +716,7 @@
         <v>36</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>40</v>
@@ -722,7 +736,7 @@
         <v>36</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="F4" s="3">
         <v>2.1</v>
@@ -742,7 +756,7 @@
         <v>36</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>50</v>
@@ -762,7 +776,7 @@
         <v>36</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>34</v>
@@ -882,7 +896,7 @@
         <v>36</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="F12" s="3">
         <v>2.1</v>
@@ -902,7 +916,7 @@
         <v>36</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="F13" s="3">
         <v>2.1</v>
@@ -922,7 +936,7 @@
         <v>36</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="F14" s="3">
         <v>2.1</v>
@@ -942,7 +956,7 @@
         <v>36</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="F15" s="3">
         <v>5</v>
@@ -962,7 +976,7 @@
         <v>36</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>36</v>
@@ -1142,7 +1156,7 @@
         <v>36</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>40</v>
@@ -1162,7 +1176,7 @@
         <v>36</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="F26" s="3">
         <v>5</v>
@@ -1182,7 +1196,7 @@
         <v>36</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>41</v>
@@ -1202,7 +1216,7 @@
         <v>36</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="F28" s="3">
         <v>2.1</v>
@@ -1222,7 +1236,7 @@
         <v>36</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="F29" s="3">
         <v>2.1</v>

</xml_diff>

<commit_message>
(#83) Visual Node Generation for Python Library Kornia
</commit_message>
<xml_diff>
--- a/mapping_common_input_java_types_full.xlsx
+++ b/mapping_common_input_java_types_full.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\59803\Auto_generation_pipeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DD732D-D111-4EF6-8A49-F7849EF2E151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26460318-29DB-4BC3-8C8B-627A36C9F9E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30" yWindow="-18120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -253,7 +253,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -276,40 +276,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -321,27 +292,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -649,17 +610,17 @@
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="H25" sqref="H25"/>
+      <selection pane="bottomLeft" activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="68.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" customWidth="1"/>
-    <col min="3" max="3" width="48.21875" customWidth="1"/>
-    <col min="4" max="4" width="25.5546875" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="14" style="3" customWidth="1"/>
+    <col min="1" max="1" width="46.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -672,10 +633,10 @@
       <c r="C1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="2" t="s">
         <v>43</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -686,19 +647,19 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="C2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="9" t="s">
         <v>40</v>
       </c>
     </row>
@@ -706,19 +667,19 @@
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="C3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="9" t="s">
         <v>40</v>
       </c>
     </row>
@@ -726,19 +687,19 @@
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="6" t="s">
+      <c r="C4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="9">
         <v>2.1</v>
       </c>
     </row>
@@ -746,19 +707,19 @@
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="6" t="s">
+      <c r="C5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="9" t="s">
         <v>50</v>
       </c>
     </row>
@@ -766,19 +727,19 @@
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="6" t="s">
+      <c r="C6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="9" t="s">
         <v>34</v>
       </c>
     </row>
@@ -786,19 +747,19 @@
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="6" t="s">
+      <c r="C7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="9" t="s">
         <v>36</v>
       </c>
     </row>
@@ -806,19 +767,19 @@
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="9" t="s">
         <v>48</v>
       </c>
     </row>
@@ -826,19 +787,19 @@
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="11" t="s">
+      <c r="C9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="9" t="s">
         <v>36</v>
       </c>
     </row>
@@ -846,19 +807,19 @@
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="11" t="s">
+      <c r="C10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="9" t="s">
         <v>36</v>
       </c>
     </row>
@@ -866,19 +827,19 @@
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="11" t="s">
+      <c r="C11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="9" t="s">
         <v>36</v>
       </c>
     </row>
@@ -886,19 +847,19 @@
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="6" t="s">
+      <c r="C12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="9">
         <v>2.1</v>
       </c>
     </row>
@@ -906,19 +867,19 @@
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="6" t="s">
+      <c r="C13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="9">
         <v>2.1</v>
       </c>
     </row>
@@ -926,19 +887,19 @@
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" s="6" t="s">
+      <c r="C14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="9">
         <v>2.1</v>
       </c>
     </row>
@@ -946,19 +907,19 @@
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="6" t="s">
+      <c r="C15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="9">
         <v>5</v>
       </c>
     </row>
@@ -966,19 +927,19 @@
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="6" t="s">
+      <c r="C16" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="9" t="s">
         <v>36</v>
       </c>
     </row>
@@ -986,19 +947,19 @@
       <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="9" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1006,19 +967,19 @@
       <c r="A18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" s="10" t="s">
+      <c r="C18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="9" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1026,19 +987,19 @@
       <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="6" t="s">
+      <c r="C19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="9" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1046,19 +1007,19 @@
       <c r="A20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="9" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1066,19 +1027,19 @@
       <c r="A21" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="6" t="s">
+      <c r="C21" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="9" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1086,19 +1047,19 @@
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E22" s="6" t="s">
+      <c r="C22" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="9" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1106,19 +1067,19 @@
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="9" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1126,19 +1087,19 @@
       <c r="A24" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E24" s="6" t="s">
+      <c r="C24" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="9" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1146,19 +1107,19 @@
       <c r="A25" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E25" s="6" t="s">
+      <c r="C25" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="9" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1166,19 +1127,19 @@
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E26" s="6" t="s">
+      <c r="C26" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="9">
         <v>5</v>
       </c>
     </row>
@@ -1186,19 +1147,19 @@
       <c r="A27" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E27" s="6" t="s">
+      <c r="C27" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="9" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1206,19 +1167,19 @@
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E28" s="6" t="s">
+      <c r="C28" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28" s="9">
         <v>2.1</v>
       </c>
     </row>
@@ -1226,24 +1187,24 @@
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E29" s="6" t="s">
+      <c r="C29" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29" s="9">
         <v>2.1</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G31" s="6"/>
+      <c r="G31" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>